<commit_message>
Add manual matches and clean status table for intersection tracking
- Added 6 confirmed manual Lotto 1 -> Master intersection matches
- Created generate_status_table.py for user-friendly status entry
- Regenerated MASTER_INTERSECTION_REPORT_CLEAN.xlsx with improved matches
- Created INTERSECTION_STATUS_TABLE.xlsx with formatted status columns

https://claude.ai/code/session_01MD92mQo6vT3XosTWnx29qJ
</commit_message>
<xml_diff>
--- a/data-import/MASTER_INTERSECTION_REPORT_CLEAN.xlsx
+++ b/data-import/MASTER_INTERSECTION_REPORT_CLEAN.xlsx
@@ -2677,7 +2677,7 @@
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr">
         <is>
-          <t>Pio XI/Anastasio II/Leone XIII</t>
+          <t>Via Anastasio II - Pio XI</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
@@ -2687,12 +2687,12 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>non passa</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
@@ -2705,7 +2705,7 @@
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>2023-09-24 00:00:00</t>
+          <t>2023-09-28 00:00:00</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr"/>
@@ -5685,17 +5685,33 @@
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.54)</t>
-        </is>
-      </c>
-      <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
+          <t>Via Cristoforo Colombo - Via Druso</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
-      <c r="AE41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>2023-08-28 00:00:00</t>
+        </is>
+      </c>
       <c r="AF41" t="inlineStr"/>
       <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="inlineStr"/>
@@ -9981,17 +9997,49 @@
       <c r="V74" t="inlineStr"/>
       <c r="W74" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.64)</t>
-        </is>
-      </c>
-      <c r="X74" t="inlineStr"/>
-      <c r="Y74" t="inlineStr"/>
-      <c r="Z74" t="inlineStr"/>
-      <c r="AA74" t="inlineStr"/>
-      <c r="AB74" t="inlineStr"/>
-      <c r="AC74" t="inlineStr"/>
-      <c r="AD74" t="inlineStr"/>
-      <c r="AE74" t="inlineStr"/>
+          <t>Piazza di porta Portese</t>
+        </is>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z74" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AB74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AD74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AE74" t="inlineStr">
+        <is>
+          <t>2023-01-31 00:00:00</t>
+        </is>
+      </c>
       <c r="AF74" t="inlineStr"/>
       <c r="AG74" t="inlineStr"/>
       <c r="AH74" t="inlineStr"/>
@@ -12239,15 +12287,35 @@
       </c>
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
-      <c r="W93" t="inlineStr"/>
-      <c r="X93" t="inlineStr"/>
-      <c r="Y93" t="inlineStr"/>
-      <c r="Z93" t="inlineStr"/>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>L.RE Diaz - Largo Mllo Diaz</t>
+        </is>
+      </c>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>parziale</t>
+        </is>
+      </c>
+      <c r="Z93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="AA93" t="inlineStr"/>
       <c r="AB93" t="inlineStr"/>
       <c r="AC93" t="inlineStr"/>
       <c r="AD93" t="inlineStr"/>
-      <c r="AE93" t="inlineStr"/>
+      <c r="AE93" t="inlineStr">
+        <is>
+          <t>2023-10-11 00:00:00</t>
+        </is>
+      </c>
       <c r="AF93" t="inlineStr"/>
       <c r="AG93" t="inlineStr"/>
       <c r="AH93" t="inlineStr"/>
@@ -12697,17 +12765,49 @@
       <c r="V97" t="inlineStr"/>
       <c r="W97" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.50)</t>
-        </is>
-      </c>
-      <c r="X97" t="inlineStr"/>
-      <c r="Y97" t="inlineStr"/>
-      <c r="Z97" t="inlineStr"/>
-      <c r="AA97" t="inlineStr"/>
-      <c r="AB97" t="inlineStr"/>
-      <c r="AC97" t="inlineStr"/>
-      <c r="AD97" t="inlineStr"/>
-      <c r="AE97" t="inlineStr"/>
+          <t>Emo - Bus</t>
+        </is>
+      </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z97" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AA97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AB97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AC97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AD97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AE97" t="inlineStr">
+        <is>
+          <t>2023-10-17 00:00:00</t>
+        </is>
+      </c>
       <c r="AF97" t="inlineStr"/>
       <c r="AG97" t="inlineStr"/>
       <c r="AH97" t="inlineStr"/>
@@ -14281,17 +14381,33 @@
       <c r="V112" t="inlineStr"/>
       <c r="W112" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.67)</t>
-        </is>
-      </c>
-      <c r="X112" t="inlineStr"/>
-      <c r="Y112" t="inlineStr"/>
-      <c r="Z112" t="inlineStr"/>
+          <t>Via Cernaia - Via Goito</t>
+        </is>
+      </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y112" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="Z112" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" t="inlineStr"/>
       <c r="AC112" t="inlineStr"/>
       <c r="AD112" t="inlineStr"/>
-      <c r="AE112" t="inlineStr"/>
+      <c r="AE112" t="inlineStr">
+        <is>
+          <t>2025-12-11 00:00:00</t>
+        </is>
+      </c>
       <c r="AF112" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
       <c r="AH112" t="inlineStr"/>
@@ -29292,7 +29408,7 @@
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr">
         <is>
-          <t>Pio XI/Anastasio II/Leone XIII</t>
+          <t>Via Anastasio II - Pio XI</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
@@ -29302,12 +29418,12 @@
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>non passa</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
@@ -29320,7 +29436,7 @@
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>2023-09-24 00:00:00</t>
+          <t>2023-09-28 00:00:00</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr"/>
@@ -32300,17 +32416,33 @@
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.54)</t>
-        </is>
-      </c>
-      <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
+          <t>Via Cristoforo Colombo - Via Druso</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="inlineStr"/>
       <c r="AD41" t="inlineStr"/>
-      <c r="AE41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>2023-08-28 00:00:00</t>
+        </is>
+      </c>
       <c r="AF41" t="inlineStr"/>
       <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="inlineStr"/>
@@ -36596,17 +36728,49 @@
       <c r="V74" t="inlineStr"/>
       <c r="W74" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.64)</t>
-        </is>
-      </c>
-      <c r="X74" t="inlineStr"/>
-      <c r="Y74" t="inlineStr"/>
-      <c r="Z74" t="inlineStr"/>
-      <c r="AA74" t="inlineStr"/>
-      <c r="AB74" t="inlineStr"/>
-      <c r="AC74" t="inlineStr"/>
-      <c r="AD74" t="inlineStr"/>
-      <c r="AE74" t="inlineStr"/>
+          <t>Piazza di porta Portese</t>
+        </is>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z74" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AB74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AD74" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AE74" t="inlineStr">
+        <is>
+          <t>2023-01-31 00:00:00</t>
+        </is>
+      </c>
       <c r="AF74" t="inlineStr"/>
       <c r="AG74" t="inlineStr"/>
       <c r="AH74" t="inlineStr"/>
@@ -38854,15 +39018,35 @@
       </c>
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
-      <c r="W93" t="inlineStr"/>
-      <c r="X93" t="inlineStr"/>
-      <c r="Y93" t="inlineStr"/>
-      <c r="Z93" t="inlineStr"/>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>L.RE Diaz - Largo Mllo Diaz</t>
+        </is>
+      </c>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>parziale</t>
+        </is>
+      </c>
+      <c r="Z93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="AA93" t="inlineStr"/>
       <c r="AB93" t="inlineStr"/>
       <c r="AC93" t="inlineStr"/>
       <c r="AD93" t="inlineStr"/>
-      <c r="AE93" t="inlineStr"/>
+      <c r="AE93" t="inlineStr">
+        <is>
+          <t>2023-10-11 00:00:00</t>
+        </is>
+      </c>
       <c r="AF93" t="inlineStr"/>
       <c r="AG93" t="inlineStr"/>
       <c r="AH93" t="inlineStr"/>
@@ -39312,17 +39496,49 @@
       <c r="V97" t="inlineStr"/>
       <c r="W97" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.50)</t>
-        </is>
-      </c>
-      <c r="X97" t="inlineStr"/>
-      <c r="Y97" t="inlineStr"/>
-      <c r="Z97" t="inlineStr"/>
-      <c r="AA97" t="inlineStr"/>
-      <c r="AB97" t="inlineStr"/>
-      <c r="AC97" t="inlineStr"/>
-      <c r="AD97" t="inlineStr"/>
-      <c r="AE97" t="inlineStr"/>
+          <t>Emo - Bus</t>
+        </is>
+      </c>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="Z97" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AA97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AB97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AC97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AD97" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="AE97" t="inlineStr">
+        <is>
+          <t>2023-10-17 00:00:00</t>
+        </is>
+      </c>
       <c r="AF97" t="inlineStr"/>
       <c r="AG97" t="inlineStr"/>
       <c r="AH97" t="inlineStr"/>
@@ -40896,17 +41112,33 @@
       <c r="V112" t="inlineStr"/>
       <c r="W112" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.67)</t>
-        </is>
-      </c>
-      <c r="X112" t="inlineStr"/>
-      <c r="Y112" t="inlineStr"/>
-      <c r="Z112" t="inlineStr"/>
+          <t>Via Cernaia - Via Goito</t>
+        </is>
+      </c>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>si</t>
+        </is>
+      </c>
+      <c r="Y112" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="Z112" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" t="inlineStr"/>
       <c r="AC112" t="inlineStr"/>
       <c r="AD112" t="inlineStr"/>
-      <c r="AE112" t="inlineStr"/>
+      <c r="AE112" t="inlineStr">
+        <is>
+          <t>2025-12-11 00:00:00</t>
+        </is>
+      </c>
       <c r="AF112" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
       <c r="AH112" t="inlineStr"/>
@@ -53877,7 +54109,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP15"/>
+  <dimension ref="A1:AP11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54100,22 +54332,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>432</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Caracalla/Colombo/Druso</t>
+          <t>Trionfale/Ipogeo degli Ottavi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>209-Caracalla/Colombo/Druso</t>
+          <t>432-Trionfale/Ipogeo degli Ottavi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1048.0</t>
+          <t>19062.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -54125,22 +54357,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tmacs</t>
+          <t>Omnia</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>Da inviare</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Ass.FM/MC</t>
+          <t>DA VRF</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -54150,7 +54382,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>AUT</t>
+          <t>Centralizzato</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
@@ -54160,26 +54392,18 @@
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Configurare AUT da remoto/Configurare AUT in lab/Sostituire AUT?!?!</t>
-        </is>
-      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>
           <t>UNCERTAIN (0.54)</t>
@@ -54208,22 +54432,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>252</t>
+          <t>434</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Portuense/Porta Portese</t>
+          <t>Battistini/Forte Braschi</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>252-Portuense/Porta Portese</t>
+          <t>434-Battistini/Forte Braschi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1053.0</t>
+          <t>19015.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -54243,12 +54467,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>Invio_12/25</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>DaFare</t>
+          <t>DA VRF</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -54256,7 +54480,11 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Centralizzato</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
@@ -54264,25 +54492,21 @@
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Idoneo</t>
-        </is>
-      </c>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.64)</t>
+          <t>UNCERTAIN (0.67)</t>
         </is>
       </c>
       <c r="X3" t="inlineStr"/>
@@ -54308,22 +54532,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>417</t>
+          <t>436</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Angelo Emo/Capolinea Bus</t>
+          <t>Trionfale/Fratelli Gualandi</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>417-Angelo Emo/Capolinea Bus</t>
+          <t>436-Trionfale/Fratelli Gualandi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18099.0</t>
+          <t>19006.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -54338,17 +54562,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>Da inviare</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>DaFare</t>
+          <t>DA VRF</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -54356,7 +54580,11 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Centralizzato</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
@@ -54364,12 +54592,12 @@
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
@@ -54378,7 +54606,7 @@
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.50)</t>
+          <t>UNCERTAIN (0.67)</t>
         </is>
       </c>
       <c r="X4" t="inlineStr"/>
@@ -54404,22 +54632,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>432</t>
+          <t>437</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Trionfale/Ipogeo degli Ottavi</t>
+          <t>Boccea/Don Carlo Gnocchi</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>432-Trionfale/Ipogeo degli Ottavi</t>
+          <t>437-Boccea/Don Carlo Gnocchi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>19062.0</t>
+          <t>18038.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -54478,7 +54706,7 @@
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.54)</t>
+          <t>UNCERTAIN (0.60)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr"/>
@@ -54504,22 +54732,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>434</t>
+          <t>438</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Battistini/Forte Braschi</t>
+          <t>Boccea/Bra</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>434-Battistini/Forte Braschi</t>
+          <t>438-Boccea/Bra</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>19015.0</t>
+          <t>18019.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -54534,12 +54762,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Invio_12/25</t>
+          <t>Da inviare</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -54554,7 +54782,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Centralizzato</t>
+          <t>Omnia</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
@@ -54567,7 +54795,7 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
@@ -54604,22 +54832,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>436</t>
+          <t>439</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Trionfale/Fratelli Gualandi</t>
+          <t>Torrevecchia/Cardinale Costantini</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>436-Trionfale/Fratelli Gualandi</t>
+          <t>439-Torrevecchia/Cardinale Costantini</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>19006.0</t>
+          <t>19028.0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -54634,7 +54862,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -54667,7 +54895,7 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
@@ -54678,7 +54906,7 @@
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.67)</t>
+          <t>UNCERTAIN (0.51)</t>
         </is>
       </c>
       <c r="X7" t="inlineStr"/>
@@ -54704,22 +54932,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>437</t>
+          <t>440</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Boccea/Don Carlo Gnocchi</t>
+          <t>Torrevecchia/Aloisi Masella</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>437-Boccea/Don Carlo Gnocchi</t>
+          <t>440-Torrevecchia/Aloisi Masella</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18038.0</t>
+          <t>19029.0</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -54734,7 +54962,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -54767,7 +54995,7 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
@@ -54778,7 +55006,7 @@
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.60)</t>
+          <t>UNCERTAIN (0.52)</t>
         </is>
       </c>
       <c r="X8" t="inlineStr"/>
@@ -54804,22 +55032,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>438</t>
+          <t>449</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Boccea/Bra</t>
+          <t>Largo del Tritone</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>438-Boccea/Bra</t>
+          <t>449-Largo del Tritone</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>18019.0</t>
+          <t>1003.0</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -54834,7 +55062,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -54852,11 +55080,7 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Omnia</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
@@ -54867,7 +55091,7 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
@@ -54878,7 +55102,7 @@
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.67)</t>
+          <t>UNCERTAIN (0.55)</t>
         </is>
       </c>
       <c r="X9" t="inlineStr"/>
@@ -54904,22 +55128,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>439</t>
+          <t>450</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Torrevecchia/Cardinale Costantini</t>
+          <t>Flaminia/Piazza dei Carracci</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>439-Torrevecchia/Cardinale Costantini</t>
+          <t>450-Flaminia/Piazza dei Carracci</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>19028.0</t>
+          <t>2092.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -54934,7 +55158,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -54952,11 +55176,7 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Centralizzato</t>
-        </is>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
@@ -54967,7 +55187,7 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr"/>
@@ -54978,7 +55198,7 @@
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.51)</t>
+          <t>UNCERTAIN (0.55)</t>
         </is>
       </c>
       <c r="X10" t="inlineStr"/>
@@ -55004,22 +55224,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>440</t>
+          <t>453</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Torrevecchia/Aloisi Masella</t>
+          <t>Piazza Cavour/Cicerone</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>440-Torrevecchia/Aloisi Masella</t>
+          <t>453-Piazza Cavour/Cicerone</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>19029.0</t>
+          <t>17114.0</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -55034,7 +55254,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -55067,7 +55287,7 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
@@ -55078,7 +55298,7 @@
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr">
         <is>
-          <t>UNCERTAIN (0.52)</t>
+          <t>UNCERTAIN (0.62)</t>
         </is>
       </c>
       <c r="X11" t="inlineStr"/>
@@ -55101,394 +55321,6 @@
       <c r="AO11" t="inlineStr"/>
       <c r="AP11" t="inlineStr"/>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>442</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Cernaia/Goito</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>442-Cernaia/Goito</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1024.0</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>M9.1</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Omnia</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Invio_12/25</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>DA VRF</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>UNCERTAIN (0.67)</t>
-        </is>
-      </c>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="inlineStr"/>
-      <c r="AM12" t="inlineStr"/>
-      <c r="AN12" t="inlineStr"/>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>449</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Largo del Tritone</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>449-Largo del Tritone</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1003.0</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>M9.1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Omnia</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Da inviare</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>DA VRF</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>UNCERTAIN (0.55)</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>450</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Flaminia/Piazza dei Carracci</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>450-Flaminia/Piazza dei Carracci</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2092.0</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>M9.1</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Omnia</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Da inviare</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>DA VRF</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>UNCERTAIN (0.55)</t>
-        </is>
-      </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="inlineStr"/>
-      <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="inlineStr"/>
-      <c r="AL14" t="inlineStr"/>
-      <c r="AM14" t="inlineStr"/>
-      <c r="AN14" t="inlineStr"/>
-      <c r="AO14" t="inlineStr"/>
-      <c r="AP14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>453</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Piazza Cavour/Cicerone</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>453-Piazza Cavour/Cicerone</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>17114.0</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>M9.1</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Omnia</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Da inviare</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>DA VRF</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Centralizzato</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>3.0</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>UNCERTAIN (0.62)</t>
-        </is>
-      </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="inlineStr"/>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>